<commit_message>
Wait added in Sp execution
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{45BD66A4-6914-48E6-9411-7B0B3DCDB353}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{19CB75D4-727A-4C5B-912E-46E502547521}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11925" windowHeight="6015" firstSheet="2" activeTab="2" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16485" windowHeight="3255" activeTab="1" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="KSIDC_CP_Login" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="EWCLeaveRequest" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A4:D21"/>
+  <oleSize ref="B1:H7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1028,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F5BEBC-63DB-4F03-9AF6-8CE69341974D}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,7 +1092,7 @@
         <v>87</v>
       </c>
       <c r="C2" s="11">
-        <v>9954327855</v>
+        <v>8080808080</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="18" t="s">
@@ -1135,7 +1135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52F80EF-30F9-4CBE-97A9-F5DB22DCED8A}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>